<commit_message>
matyu65@hotmail.com 14/09/2025 Agregacion de casos , agregar la propuesta de casos
</commit_message>
<xml_diff>
--- a/Prueba_Tecnica_Siigo/src/test/resources/datadriver/crearcliente/crear_cliente.xlsx
+++ b/Prueba_Tecnica_Siigo/src/test/resources/datadriver/crearcliente/crear_cliente.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matyu\Documents\Siigo\Prueba_Tecnica_Siigo\src\test\resources\datadriver\crearcliente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540F5DA-6EB4-47ED-BCE7-FA64D5FC659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F11D566-2CFE-47E2-B16D-43078D7B383D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>usuario</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>retoautomationsiigo@yopmail.com</t>
+  </si>
+  <si>
+    <t>opcionPrincipal</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Tip_documento</t>
+  </si>
+  <si>
+    <t>Cédula de ciudadanía</t>
   </si>
 </sst>
 </file>
@@ -383,37 +395,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>